<commit_message>
agregué nombres de historia de usuario productbacklog
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -142,9 +142,6 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -153,6 +150,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -437,7 +437,7 @@
   <dimension ref="B2:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -450,205 +450,205 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
     </row>
     <row r="4" spans="2:10" ht="26.25" customHeight="1">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="39.4" customHeight="1">
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>7</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>6</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <f>AVERAGE(F5:G5)</f>
         <v>6.5</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>1</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="59.25" customHeight="1">
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="4">
-        <v>4</v>
-      </c>
-      <c r="G6" s="4">
-        <v>4</v>
-      </c>
-      <c r="H6" s="4">
+      <c r="F6" s="3">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3">
+        <v>4</v>
+      </c>
+      <c r="H6" s="3">
         <f>AVERAGE(F6:G6)</f>
         <v>4</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>1</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="57.75" customHeight="1">
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>3</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>3</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <f>AVERAGE(F7:G7)</f>
         <v>3</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>1</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="56.25" customHeight="1">
-      <c r="B8" s="2">
-        <v>4</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="4">
-        <v>4</v>
-      </c>
-      <c r="G8" s="4">
-        <v>4</v>
-      </c>
-      <c r="H8" s="4">
+      <c r="F8" s="3">
+        <v>4</v>
+      </c>
+      <c r="G8" s="3">
+        <v>4</v>
+      </c>
+      <c r="H8" s="3">
         <f>AVERAGE(F8:G8)</f>
         <v>4</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>1</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="69.75" customHeight="1">
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>5</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>8</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>9</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <f>AVERAGE(F9:G9)</f>
         <v>8.5</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>1</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="3">
         <v>5</v>
       </c>
     </row>

</xml_diff>